<commit_message>
Solving Advertisement-mix with Linear Programming
</commit_message>
<xml_diff>
--- a/prescriptive-analytics/marketing-mix.xlsx
+++ b/prescriptive-analytics/marketing-mix.xlsx
@@ -9,12 +9,71 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" tabRatio="650" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="marketing-mix" sheetId="2" r:id="rId1"/>
-    <sheet name="Marketing Linear Programmings" sheetId="1" r:id="rId2"/>
+    <sheet name="Answer Report 1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sensitivity Report 1" sheetId="4" r:id="rId3"/>
+    <sheet name="Limits Report 1" sheetId="5" r:id="rId4"/>
+    <sheet name="Marketing Linear Programmings" sheetId="1" r:id="rId5"/>
   </sheets>
+  <definedNames>
+    <definedName name="BudgetAvailable">'Marketing Linear Programmings'!$J$8:$J$9</definedName>
+    <definedName name="BudgetSpend">'Marketing Linear Programmings'!$H$8:$H$9</definedName>
+    <definedName name="CostPerAd">'Marketing Linear Programmings'!$E$8:$G$9</definedName>
+    <definedName name="CouponRedemptionPerAd">'Marketing Linear Programmings'!$E$16:$G$16</definedName>
+    <definedName name="ExposurePerAd">'Marketing Linear Programmings'!$E$5:$G$5</definedName>
+    <definedName name="MaxTVSpots">'Marketing Linear Programmings'!$E$21</definedName>
+    <definedName name="MinimumAcceptable">'Marketing Linear Programmings'!$J$12:$J$13</definedName>
+    <definedName name="NumberOfAds">'Marketing Linear Programmings'!$E$19:$G$19</definedName>
+    <definedName name="NumberReachedPerAd">'Marketing Linear Programmings'!$E$12:$G$13</definedName>
+    <definedName name="RequiredAmount">'Marketing Linear Programmings'!$J$16</definedName>
+    <definedName name="solver_adj" localSheetId="4" hidden="1">'Marketing Linear Programmings'!$E$19:$G$19</definedName>
+    <definedName name="solver_cvg" localSheetId="4" hidden="1">0.0001</definedName>
+    <definedName name="solver_drv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_eng" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_est" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_itr" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_lhs1" localSheetId="4" hidden="1">'Marketing Linear Programmings'!$H$8:$H$9</definedName>
+    <definedName name="solver_lhs2" localSheetId="4" hidden="1">'Marketing Linear Programmings'!$E$19</definedName>
+    <definedName name="solver_lhs3" localSheetId="4" hidden="1">'Marketing Linear Programmings'!$H$12:$H$13</definedName>
+    <definedName name="solver_lhs4" localSheetId="4" hidden="1">'Marketing Linear Programmings'!$H$16</definedName>
+    <definedName name="solver_mip" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_mni" localSheetId="4" hidden="1">30</definedName>
+    <definedName name="solver_mrt" localSheetId="4" hidden="1">0.075</definedName>
+    <definedName name="solver_msl" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_neg" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_nod" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_num" localSheetId="4" hidden="1">4</definedName>
+    <definedName name="solver_nwt" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_opt" localSheetId="4" hidden="1">'Marketing Linear Programmings'!$J$22</definedName>
+    <definedName name="solver_pre" localSheetId="4" hidden="1">0.000001</definedName>
+    <definedName name="solver_rbv" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel1" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel2" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_rel3" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="solver_rel4" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rhs1" localSheetId="4" hidden="1">BudgetAvailable</definedName>
+    <definedName name="solver_rhs2" localSheetId="4" hidden="1">MaxTVSpots</definedName>
+    <definedName name="solver_rhs3" localSheetId="4" hidden="1">MinimumAcceptable</definedName>
+    <definedName name="solver_rhs4" localSheetId="4" hidden="1">RequiredAmount</definedName>
+    <definedName name="solver_rlx" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_rsd" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_scl" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_sho" localSheetId="3" hidden="1">2</definedName>
+    <definedName name="solver_sho" localSheetId="4" hidden="1">2</definedName>
+    <definedName name="solver_ssz" localSheetId="4" hidden="1">100</definedName>
+    <definedName name="solver_tim" localSheetId="4" hidden="1">2147483647</definedName>
+    <definedName name="solver_tol" localSheetId="4" hidden="1">0.01</definedName>
+    <definedName name="solver_typ" localSheetId="4" hidden="1">1</definedName>
+    <definedName name="solver_val" localSheetId="4" hidden="1">0</definedName>
+    <definedName name="solver_ver" localSheetId="4" hidden="1">3</definedName>
+    <definedName name="TotalExposures">'Marketing Linear Programmings'!$J$22</definedName>
+    <definedName name="TotalReached">'Marketing Linear Programmings'!$H$12:$H$13</definedName>
+    <definedName name="TotalRedeemed">'Marketing Linear Programmings'!$H$16</definedName>
+    <definedName name="TVSpots">'Marketing Linear Programmings'!$E$19</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -26,7 +85,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="147">
   <si>
     <t>Adevertising-Campaign-Mix Optimization</t>
   </si>
@@ -188,14 +247,301 @@
   </si>
   <si>
     <t>Social Media Commercial</t>
+  </si>
+  <si>
+    <t>(In Dollars)</t>
+  </si>
+  <si>
+    <t>Expected No. of Exposures</t>
+  </si>
+  <si>
+    <t>Coupon Redemption Table</t>
+  </si>
+  <si>
+    <t>Coupon Redemtion</t>
+  </si>
+  <si>
+    <t>Requirement</t>
+  </si>
+  <si>
+    <t>Target Category Table</t>
+  </si>
+  <si>
+    <t>(in Millions)</t>
+  </si>
+  <si>
+    <t>Target Category</t>
+  </si>
+  <si>
+    <t>Objective:</t>
+  </si>
+  <si>
+    <t>Maximize the Target audience Reach with given constraints</t>
+  </si>
+  <si>
+    <t>J8:J9</t>
+  </si>
+  <si>
+    <t>H8:H9</t>
+  </si>
+  <si>
+    <t>E8:G9</t>
+  </si>
+  <si>
+    <t>E16:G16</t>
+  </si>
+  <si>
+    <t>E5:G5</t>
+  </si>
+  <si>
+    <t>E21</t>
+  </si>
+  <si>
+    <t>J12:13</t>
+  </si>
+  <si>
+    <t>E19:G19</t>
+  </si>
+  <si>
+    <t>E12:G13</t>
+  </si>
+  <si>
+    <t>J16</t>
+  </si>
+  <si>
+    <t>J22</t>
+  </si>
+  <si>
+    <t>H12:H13</t>
+  </si>
+  <si>
+    <t>H16</t>
+  </si>
+  <si>
+    <t>E19</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Answer Report</t>
+  </si>
+  <si>
+    <t>Worksheet: [marketing-mix.xlsx]Marketing Linear Programmings</t>
+  </si>
+  <si>
+    <t>Report Created: 3/21/2019 1:45:16 AM</t>
+  </si>
+  <si>
+    <t>Result: Solver found a solution.  All Constraints and optimality conditions are satisfied.</t>
+  </si>
+  <si>
+    <t>Solver Engine</t>
+  </si>
+  <si>
+    <t>Engine: Simplex LP</t>
+  </si>
+  <si>
+    <t>Solution Time: 0.032 Seconds.</t>
+  </si>
+  <si>
+    <t>Iterations: 5 Subproblems: 0</t>
+  </si>
+  <si>
+    <t>Solver Options</t>
+  </si>
+  <si>
+    <t>Max Time Unlimited,  Iterations Unlimited, Precision 0.000001, Use Automatic Scaling</t>
+  </si>
+  <si>
+    <t>Max Subproblems Unlimited, Max Integer Sols Unlimited, Integer Tolerance 1%, Assume NonNegative</t>
+  </si>
+  <si>
+    <t>Objective Cell (Max)</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Original Value</t>
+  </si>
+  <si>
+    <t>Final Value</t>
+  </si>
+  <si>
+    <t>Variable Cells</t>
+  </si>
+  <si>
+    <t>Integer</t>
+  </si>
+  <si>
+    <t>Constraints</t>
+  </si>
+  <si>
+    <t>Cell Value</t>
+  </si>
+  <si>
+    <t>Formula</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Slack</t>
+  </si>
+  <si>
+    <t>$J$22</t>
+  </si>
+  <si>
+    <t>$E$19</t>
+  </si>
+  <si>
+    <t>Contin</t>
+  </si>
+  <si>
+    <t>$F$19</t>
+  </si>
+  <si>
+    <t>Number of Advertisements Magazine</t>
+  </si>
+  <si>
+    <t>$G$19</t>
+  </si>
+  <si>
+    <t>Number of Advertisements Social Media Adds</t>
+  </si>
+  <si>
+    <t>$H$8</t>
+  </si>
+  <si>
+    <t>Advertising Budget Budget Spent</t>
+  </si>
+  <si>
+    <t>$H$8&lt;=$J$8</t>
+  </si>
+  <si>
+    <t>Not Binding</t>
+  </si>
+  <si>
+    <t>$H$9</t>
+  </si>
+  <si>
+    <t>Planning Budget Budget Spent</t>
+  </si>
+  <si>
+    <t>$H$9&lt;=$J$9</t>
+  </si>
+  <si>
+    <t>Binding</t>
+  </si>
+  <si>
+    <t>$H$12</t>
+  </si>
+  <si>
+    <t>Young Children Total Reached</t>
+  </si>
+  <si>
+    <t>$H$12&gt;=$J$12</t>
+  </si>
+  <si>
+    <t>$H$13</t>
+  </si>
+  <si>
+    <t>Adults Total Reached</t>
+  </si>
+  <si>
+    <t>$H$13&gt;=$J$13</t>
+  </si>
+  <si>
+    <t>$H$16</t>
+  </si>
+  <si>
+    <t>$H$16=$J$16</t>
+  </si>
+  <si>
+    <t>$E$19&lt;=$E$21</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Sensitivity Report</t>
+  </si>
+  <si>
+    <t>Final</t>
+  </si>
+  <si>
+    <t>Value</t>
+  </si>
+  <si>
+    <t>Reduced</t>
+  </si>
+  <si>
+    <t>Cost</t>
+  </si>
+  <si>
+    <t>Objective</t>
+  </si>
+  <si>
+    <t>Coefficient</t>
+  </si>
+  <si>
+    <t>Allowable</t>
+  </si>
+  <si>
+    <t>Increase</t>
+  </si>
+  <si>
+    <t>Decrease</t>
+  </si>
+  <si>
+    <t>Shadow</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Constraint</t>
+  </si>
+  <si>
+    <t>R.H. Side</t>
+  </si>
+  <si>
+    <t>Microsoft Excel 16.0 Limits Report</t>
+  </si>
+  <si>
+    <t>Variable</t>
+  </si>
+  <si>
+    <t>Lower</t>
+  </si>
+  <si>
+    <t>Limit</t>
+  </si>
+  <si>
+    <t>Result</t>
+  </si>
+  <si>
+    <t>Upper</t>
+  </si>
+  <si>
+    <t>&lt;=</t>
+  </si>
+  <si>
+    <t>&gt;=</t>
+  </si>
+  <si>
+    <t>===</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -209,8 +555,23 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color indexed="18"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -253,8 +614,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="7">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -328,13 +701,91 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="23"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="23"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -355,7 +806,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
@@ -364,6 +814,38 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -650,48 +1132,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:E6"/>
+  <dimension ref="B2:F25"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.42578125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="20.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B2" t="s">
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
         <v>49</v>
       </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
+      <c r="C2" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="19" t="s">
         <v>50</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="19" t="s">
         <v>51</v>
       </c>
-      <c r="D4" t="s">
+      <c r="D4" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="19" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="20" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
+      <c r="C5" s="20">
+        <v>300000</v>
+      </c>
+      <c r="D5" s="20">
+        <v>150000</v>
+      </c>
+      <c r="E5" s="20">
+        <v>100000</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
         <v>7</v>
       </c>
+      <c r="C6" s="20">
+        <v>90000</v>
+      </c>
+      <c r="D6" s="20">
+        <v>30000</v>
+      </c>
+      <c r="E6" s="20">
+        <v>40000</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="C7" s="20">
+        <v>1300000</v>
+      </c>
+      <c r="D7" s="20">
+        <v>600000</v>
+      </c>
+      <c r="E7" s="20">
+        <v>500000</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="C14" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E14" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F14" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C15" s="22">
+        <v>0</v>
+      </c>
+      <c r="D15" s="20">
+        <v>40000</v>
+      </c>
+      <c r="E15" s="20">
+        <v>120000</v>
+      </c>
+      <c r="F15" s="23">
+        <v>1490000</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="C20" s="19" t="s">
+        <v>51</v>
+      </c>
+      <c r="D20" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="E20" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="19" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="20" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="20">
+        <v>1.2</v>
+      </c>
+      <c r="D21" s="20">
+        <v>0.1</v>
+      </c>
+      <c r="E21" s="20">
+        <v>0</v>
+      </c>
+      <c r="F21" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="20" t="s">
+        <v>11</v>
+      </c>
+      <c r="C22" s="20">
+        <v>0.5</v>
+      </c>
+      <c r="D22" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="E22" s="20">
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="23">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="24" t="s">
+        <v>62</v>
+      </c>
+      <c r="C25" s="24" t="s">
+        <v>63</v>
+      </c>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -700,10 +1329,895 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G35"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.42578125" customWidth="1"/>
+    <col min="7" max="7" width="5.42578125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="25" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A6" s="25"/>
+      <c r="B6" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A7" s="25"/>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="A8" s="25"/>
+      <c r="B8" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="25" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" collapsed="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D16" s="30">
+        <v>0</v>
+      </c>
+      <c r="E16" s="30">
+        <v>16175</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D20" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>92</v>
+      </c>
+      <c r="F20" s="27" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B21" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C21" s="33"/>
+      <c r="D21" s="33"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+    </row>
+    <row r="22" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B22" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C22" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" s="31">
+        <v>0</v>
+      </c>
+      <c r="E22" s="31">
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="F22" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C23" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D23" s="31">
+        <v>0</v>
+      </c>
+      <c r="E23" s="31">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="F23" s="29" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C24" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D24" s="30">
+        <v>0</v>
+      </c>
+      <c r="E24" s="30">
+        <v>7.7499999999999991</v>
+      </c>
+      <c r="F24" s="26" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B25" s="28"/>
+      <c r="C25" s="28"/>
+      <c r="D25" s="32"/>
+      <c r="E25" s="32"/>
+      <c r="F25" s="28"/>
+    </row>
+    <row r="28" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="E29" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="F29" s="27" t="s">
+        <v>98</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B30" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C30" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D30" s="31">
+        <v>3775</v>
+      </c>
+      <c r="E30" s="29" t="s">
+        <v>109</v>
+      </c>
+      <c r="F30" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="G30" s="29">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B31" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C31" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D31" s="31">
+        <v>1000</v>
+      </c>
+      <c r="E31" s="29" t="s">
+        <v>113</v>
+      </c>
+      <c r="F31" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G31" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B32" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C32" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="D32" s="31">
+        <v>4.9999999999999982</v>
+      </c>
+      <c r="E32" s="29" t="s">
+        <v>117</v>
+      </c>
+      <c r="F32" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G32" s="31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B33" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C33" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D33" s="31">
+        <v>5.85</v>
+      </c>
+      <c r="E33" s="29" t="s">
+        <v>120</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>110</v>
+      </c>
+      <c r="G33" s="31">
+        <v>0.84999999999999964</v>
+      </c>
+    </row>
+    <row r="34" spans="2:7" x14ac:dyDescent="0.25">
+      <c r="B34" s="29" t="s">
+        <v>121</v>
+      </c>
+      <c r="C34" s="29" t="s">
+        <v>35</v>
+      </c>
+      <c r="D34" s="31">
+        <v>1490</v>
+      </c>
+      <c r="E34" s="29" t="s">
+        <v>122</v>
+      </c>
+      <c r="F34" s="29" t="s">
+        <v>114</v>
+      </c>
+      <c r="G34" s="29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B35" s="26" t="s">
+        <v>101</v>
+      </c>
+      <c r="C35" s="26" t="s">
+        <v>36</v>
+      </c>
+      <c r="D35" s="30">
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>123</v>
+      </c>
+      <c r="F35" s="26" t="s">
+        <v>110</v>
+      </c>
+      <c r="G35" s="26">
+        <v>2.0000000000000018</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H22"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="12.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="12" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B7" s="35"/>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>127</v>
+      </c>
+      <c r="F7" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="H7" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D8" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E8" s="36" t="s">
+        <v>128</v>
+      </c>
+      <c r="F8" s="36" t="s">
+        <v>130</v>
+      </c>
+      <c r="G8" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H8" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B9" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+    </row>
+    <row r="10" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C10" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D10" s="29">
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="E10" s="29">
+        <v>0</v>
+      </c>
+      <c r="F10" s="29">
+        <v>1300</v>
+      </c>
+      <c r="G10" s="29">
+        <v>1040</v>
+      </c>
+      <c r="H10" s="29">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C11" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D11" s="29">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="E11" s="29">
+        <v>0</v>
+      </c>
+      <c r="F11" s="29">
+        <v>600</v>
+      </c>
+      <c r="G11" s="29">
+        <v>1E+30</v>
+      </c>
+      <c r="H11" s="29">
+        <v>192.59259259259258</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C12" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D12" s="26">
+        <v>7.7499999999999991</v>
+      </c>
+      <c r="E12" s="26">
+        <v>0</v>
+      </c>
+      <c r="F12" s="26">
+        <v>500</v>
+      </c>
+      <c r="G12" s="26">
+        <v>577.77777777777771</v>
+      </c>
+      <c r="H12" s="26">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="28"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="28"/>
+      <c r="E13" s="28"/>
+      <c r="F13" s="28"/>
+      <c r="G13" s="28"/>
+      <c r="H13" s="28"/>
+    </row>
+    <row r="15" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="B16" s="35"/>
+      <c r="C16" s="35"/>
+      <c r="D16" s="35" t="s">
+        <v>125</v>
+      </c>
+      <c r="E16" s="35" t="s">
+        <v>134</v>
+      </c>
+      <c r="F16" s="35" t="s">
+        <v>136</v>
+      </c>
+      <c r="G16" s="35" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" s="35" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B17" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C17" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D17" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="E17" s="36" t="s">
+        <v>135</v>
+      </c>
+      <c r="F17" s="36" t="s">
+        <v>137</v>
+      </c>
+      <c r="G17" s="36" t="s">
+        <v>132</v>
+      </c>
+      <c r="H17" s="36" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B18" s="29" t="s">
+        <v>107</v>
+      </c>
+      <c r="C18" s="29" t="s">
+        <v>108</v>
+      </c>
+      <c r="D18" s="29">
+        <v>3775</v>
+      </c>
+      <c r="E18" s="29">
+        <v>0</v>
+      </c>
+      <c r="F18" s="29">
+        <v>4000</v>
+      </c>
+      <c r="G18" s="29">
+        <v>1E+30</v>
+      </c>
+      <c r="H18" s="29">
+        <v>224.99999999999983</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="29" t="s">
+        <v>111</v>
+      </c>
+      <c r="C19" s="29" t="s">
+        <v>112</v>
+      </c>
+      <c r="D19" s="29">
+        <v>1000</v>
+      </c>
+      <c r="E19" s="29">
+        <v>35.454545454545467</v>
+      </c>
+      <c r="F19" s="29">
+        <v>1000</v>
+      </c>
+      <c r="G19" s="29">
+        <v>22.499999999999972</v>
+      </c>
+      <c r="H19" s="29">
+        <v>84.999999999999929</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="29" t="s">
+        <v>115</v>
+      </c>
+      <c r="C20" s="29" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="29">
+        <v>4.9999999999999982</v>
+      </c>
+      <c r="E20" s="29">
+        <v>-1575.7575757575769</v>
+      </c>
+      <c r="F20" s="29">
+        <v>5</v>
+      </c>
+      <c r="G20" s="29">
+        <v>1.3200000000000003</v>
+      </c>
+      <c r="H20" s="29">
+        <v>0.44999999999999929</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="29" t="s">
+        <v>118</v>
+      </c>
+      <c r="C21" s="29" t="s">
+        <v>119</v>
+      </c>
+      <c r="D21" s="29">
+        <v>5.85</v>
+      </c>
+      <c r="E21" s="29">
+        <v>0</v>
+      </c>
+      <c r="F21" s="29">
+        <v>5</v>
+      </c>
+      <c r="G21" s="29">
+        <v>0.84999999999999942</v>
+      </c>
+      <c r="H21" s="29">
+        <v>1E+30</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="26" t="s">
+        <v>121</v>
+      </c>
+      <c r="C22" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="D22" s="26">
+        <v>1490</v>
+      </c>
+      <c r="E22" s="26">
+        <v>-7.6515151515151567</v>
+      </c>
+      <c r="F22" s="26">
+        <v>1490</v>
+      </c>
+      <c r="G22" s="26">
+        <v>384.99999999999977</v>
+      </c>
+      <c r="H22" s="26">
+        <v>89.999999999999872</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J17"/>
+  <sheetViews>
+    <sheetView showGridLines="0" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" outlineLevelRow="1" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="2.28515625" customWidth="1"/>
+    <col min="2" max="2" width="6.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="42.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.140625" customWidth="1"/>
+    <col min="5" max="5" width="2.28515625" customWidth="1"/>
+    <col min="6" max="6" width="6.42578125" customWidth="1"/>
+    <col min="7" max="7" width="9.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="2.28515625" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" customWidth="1"/>
+    <col min="10" max="10" width="9.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A1" s="25" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A2" s="25" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A3" s="25" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B6" s="35"/>
+      <c r="C6" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="D6" s="35"/>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="36" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B8" s="26" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="26" t="s">
+        <v>33</v>
+      </c>
+      <c r="D8" s="30">
+        <v>16175</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="35"/>
+      <c r="C11" s="35" t="s">
+        <v>139</v>
+      </c>
+      <c r="D11" s="35"/>
+      <c r="F11" s="35" t="s">
+        <v>140</v>
+      </c>
+      <c r="G11" s="35" t="s">
+        <v>129</v>
+      </c>
+      <c r="I11" s="35" t="s">
+        <v>143</v>
+      </c>
+      <c r="J11" s="35" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B12" s="36" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="36" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="36" t="s">
+        <v>126</v>
+      </c>
+      <c r="F12" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="G12" s="36" t="s">
+        <v>142</v>
+      </c>
+      <c r="I12" s="36" t="s">
+        <v>141</v>
+      </c>
+      <c r="J12" s="36" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="34" t="s">
+        <v>30</v>
+      </c>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="I13" s="33"/>
+      <c r="J13" s="33"/>
+    </row>
+    <row r="14" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B14" s="29" t="s">
+        <v>101</v>
+      </c>
+      <c r="C14" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="D14" s="31">
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="F14" s="31">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="G14" s="31">
+        <v>16175.000000000002</v>
+      </c>
+      <c r="I14" s="31">
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="J14" s="31">
+        <v>16175.000000000002</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" hidden="1" outlineLevel="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="C15" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="D15" s="31">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="F15" s="31">
+        <v>14.000000000000002</v>
+      </c>
+      <c r="G15" s="31">
+        <v>16175</v>
+      </c>
+      <c r="I15" s="31">
+        <v>14.000000000000002</v>
+      </c>
+      <c r="J15" s="31">
+        <v>16175</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" ht="15.75" hidden="1" outlineLevel="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B16" s="26" t="s">
+        <v>105</v>
+      </c>
+      <c r="C16" s="26" t="s">
+        <v>106</v>
+      </c>
+      <c r="D16" s="30">
+        <v>7.7499999999999991</v>
+      </c>
+      <c r="F16" s="30">
+        <v>7.75</v>
+      </c>
+      <c r="G16" s="30">
+        <v>16175</v>
+      </c>
+      <c r="I16" s="30">
+        <v>7.75</v>
+      </c>
+      <c r="J16" s="30">
+        <v>16175</v>
+      </c>
+    </row>
+    <row r="17" spans="2:10" collapsed="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="28"/>
+      <c r="C17" s="28"/>
+      <c r="D17" s="32"/>
+      <c r="F17" s="32"/>
+      <c r="G17" s="32"/>
+      <c r="I17" s="32"/>
+      <c r="J17" s="32"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B2:J40"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H31" sqref="H31"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E20" sqref="E20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -717,13 +2231,13 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="38.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="2"/>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2"/>
+      <c r="E2" s="2"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="4" spans="2:10" x14ac:dyDescent="0.25">
       <c r="E4" t="s">
@@ -737,18 +2251,18 @@
       </c>
     </row>
     <row r="5" spans="2:10" ht="26.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="6"/>
-      <c r="D5" s="6"/>
-      <c r="E5" s="4">
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="5">
         <v>1300</v>
       </c>
-      <c r="F5" s="5">
+      <c r="F5" s="6">
         <v>600</v>
       </c>
-      <c r="G5" s="5">
+      <c r="G5" s="6">
         <v>500</v>
       </c>
     </row>
@@ -764,40 +2278,54 @@
       </c>
     </row>
     <row r="8" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="3">
+      <c r="C8" s="7"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="4">
         <v>300</v>
       </c>
-      <c r="F8" s="3">
+      <c r="F8" s="4">
         <v>150</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="4">
         <v>100</v>
       </c>
-      <c r="J8" s="9">
+      <c r="H8" s="4">
+        <f>SUMPRODUCT(E8:G8,NumberOfAds)</f>
+        <v>3775</v>
+      </c>
+      <c r="I8" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="J8" s="10">
         <v>4000</v>
       </c>
     </row>
     <row r="9" spans="2:10" x14ac:dyDescent="0.25">
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="6"/>
-      <c r="E9" s="3">
+      <c r="C9" s="7"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="4">
         <v>90</v>
       </c>
-      <c r="F9" s="3">
+      <c r="F9" s="4">
         <v>30</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="4">
         <v>40</v>
       </c>
-      <c r="J9" s="9">
+      <c r="H9" s="4">
+        <f>SUMPRODUCT(E9:G9,NumberOfAds)</f>
+        <v>1000</v>
+      </c>
+      <c r="I9" s="25" t="s">
+        <v>144</v>
+      </c>
+      <c r="J9" s="10">
         <v>1000</v>
       </c>
     </row>
@@ -816,19 +2344,23 @@
       <c r="B12" t="s">
         <v>10</v>
       </c>
-      <c r="E12" s="3">
+      <c r="E12" s="4">
         <v>1.2</v>
       </c>
-      <c r="F12" s="3">
+      <c r="F12" s="4">
         <v>0.1</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="4">
         <v>0</v>
       </c>
-      <c r="H12" s="8">
-        <v>5</v>
-      </c>
-      <c r="J12" s="9">
+      <c r="H12" s="9">
+        <f>SUMPRODUCT(E12:G12,NumberOfAds)</f>
+        <v>4.9999999999999982</v>
+      </c>
+      <c r="I12" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="J12" s="10">
         <v>5</v>
       </c>
     </row>
@@ -836,19 +2368,23 @@
       <c r="B13" t="s">
         <v>11</v>
       </c>
-      <c r="E13" s="3">
+      <c r="E13" s="4">
         <v>0.5</v>
       </c>
-      <c r="F13" s="3">
+      <c r="F13" s="4">
         <v>0.2</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="4">
         <v>0.2</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="9">
+        <f>SUMPRODUCT(E13:G13,NumberOfAds)</f>
         <v>5.85</v>
       </c>
-      <c r="J13" s="9">
+      <c r="I13" s="25" t="s">
+        <v>145</v>
+      </c>
+      <c r="J13" s="10">
         <v>5</v>
       </c>
     </row>
@@ -870,22 +2406,26 @@
       </c>
     </row>
     <row r="16" spans="2:10" ht="30" x14ac:dyDescent="0.25">
-      <c r="B16" s="7" t="s">
+      <c r="B16" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="E16" s="3">
+      <c r="E16" s="4">
         <v>0</v>
       </c>
-      <c r="F16" s="3">
+      <c r="F16" s="4">
         <v>40</v>
       </c>
-      <c r="G16" s="3">
+      <c r="G16" s="4">
         <v>120</v>
       </c>
-      <c r="H16" s="8">
+      <c r="H16" s="9">
+        <f>SUMPRODUCT(CouponRedemptionPerAd,NumberOfAds)</f>
         <v>1490</v>
       </c>
-      <c r="J16" s="9">
+      <c r="I16" s="38" t="s">
+        <v>146</v>
+      </c>
+      <c r="J16" s="10">
         <v>1490</v>
       </c>
     </row>
@@ -904,11 +2444,20 @@
       <c r="B19" t="s">
         <v>18</v>
       </c>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
+      <c r="E19" s="9">
+        <v>2.9999999999999982</v>
+      </c>
+      <c r="F19" s="9">
+        <v>14.000000000000004</v>
+      </c>
+      <c r="G19" s="9">
+        <v>7.7499999999999991</v>
+      </c>
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.25">
+      <c r="E20" s="25" t="s">
+        <v>144</v>
+      </c>
       <c r="J20" t="s">
         <v>20</v>
       </c>
@@ -917,12 +2466,15 @@
       <c r="B21" t="s">
         <v>19</v>
       </c>
-      <c r="E21" s="9">
+      <c r="E21" s="10">
         <v>5</v>
       </c>
     </row>
     <row r="22" spans="2:10" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="J22" s="10"/>
+      <c r="J22" s="37">
+        <f>SUMPRODUCT(ExposurePerAd,NumberOfAds)</f>
+        <v>16175</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -941,7 +2493,9 @@
       <c r="B27" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C27" s="12"/>
+      <c r="C27" s="12" t="s">
+        <v>64</v>
+      </c>
       <c r="F27" s="11" t="s">
         <v>39</v>
       </c>
@@ -953,7 +2507,9 @@
       <c r="B28" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C28" s="12"/>
+      <c r="C28" s="12" t="s">
+        <v>65</v>
+      </c>
       <c r="F28" s="11" t="s">
         <v>41</v>
       </c>
@@ -965,7 +2521,9 @@
       <c r="B29" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="12"/>
+      <c r="C29" s="12" t="s">
+        <v>66</v>
+      </c>
       <c r="F29" s="11" t="s">
         <v>42</v>
       </c>
@@ -977,7 +2535,9 @@
       <c r="B30" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C30" s="12"/>
+      <c r="C30" s="12" t="s">
+        <v>67</v>
+      </c>
       <c r="F30" s="17" t="s">
         <v>43</v>
       </c>
@@ -987,7 +2547,9 @@
       <c r="B31" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="C31" s="12"/>
+      <c r="C31" s="12" t="s">
+        <v>68</v>
+      </c>
       <c r="F31" s="17" t="s">
         <v>44</v>
       </c>
@@ -997,7 +2559,9 @@
       <c r="B32" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="C32" s="12"/>
+      <c r="C32" s="12" t="s">
+        <v>69</v>
+      </c>
       <c r="F32" s="11" t="s">
         <v>45</v>
       </c>
@@ -1007,7 +2571,9 @@
       <c r="B33" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C33" s="12"/>
+      <c r="C33" s="12" t="s">
+        <v>70</v>
+      </c>
       <c r="F33" s="17" t="s">
         <v>46</v>
       </c>
@@ -1017,7 +2583,9 @@
       <c r="B34" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="12"/>
+      <c r="C34" s="12" t="s">
+        <v>71</v>
+      </c>
       <c r="F34" s="17" t="s">
         <v>47</v>
       </c>
@@ -1027,7 +2595,9 @@
       <c r="B35" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="12"/>
+      <c r="C35" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="F35" s="11" t="s">
         <v>48</v>
       </c>
@@ -1037,7 +2607,9 @@
       <c r="B36" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="C36" s="12"/>
+      <c r="C36" s="12" t="s">
+        <v>73</v>
+      </c>
       <c r="F36" s="13"/>
       <c r="G36" s="14"/>
     </row>
@@ -1045,25 +2617,33 @@
       <c r="B37" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="12"/>
+      <c r="C37" s="12" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="38" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B38" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C38" s="12"/>
+      <c r="C38" s="12" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="39" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B39" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="12"/>
+      <c r="C39" s="12" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="40" spans="2:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B40" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="14"/>
+      <c r="C40" s="14" t="s">
+        <v>77</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>